<commit_message>
add minimal test plan to all profiles
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.pain.xlsx
+++ b/docs/StructureDefinition-VA.MHV.pain.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$67</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="482">
   <si>
     <t>Path</t>
   </si>
@@ -999,7 +999,7 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantity
+    <t xml:space="preserve">integer
 </t>
   </si>
   <si>
@@ -1031,135 +1031,7 @@
     <t>363714003 |Interprets|</t>
   </si>
   <si>
-    <t>valueQuantity</t>
-  </si>
-  <si>
-    <t>Observation.value[x].id</t>
-  </si>
-  <si>
-    <t>Observation.value[x].extension</t>
-  </si>
-  <si>
-    <t>Observation.value[x].value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal
-</t>
-  </si>
-  <si>
-    <t>Numerical value (with implicit precision)</t>
-  </si>
-  <si>
-    <t>The value of the measured amount. The value includes an implicit precision in the presentation of the value.</t>
-  </si>
-  <si>
-    <t>The implicit precision in the value should always be honored. Monetary values have their own rules for handling precision (refer to standard accounting text books).</t>
-  </si>
-  <si>
-    <t>Precision is handled implicitly in almost all cases of measurement.</t>
-  </si>
-  <si>
-    <t>Quantity.value</t>
-  </si>
-  <si>
-    <t>SN.2  / CQ - N/A</t>
-  </si>
-  <si>
-    <t>PQ.value, CO.value, MO.value, IVL.high or IVL.low depending on the value</t>
-  </si>
-  <si>
-    <t>Observation.value[x].comparator</t>
-  </si>
-  <si>
-    <t>&lt; | &lt;= | &gt;= | &gt; - how to understand the value</t>
-  </si>
-  <si>
-    <t>How the value should be understood and represented - whether the actual value is greater or less than the stated value due to measurement issues; e.g. if the comparator is "&lt;" , then the real value is &lt; stated value.</t>
-  </si>
-  <si>
-    <t>Need a framework for handling measures where the value is &lt;5ug/L or &gt;400mg/L due to the limitations of measuring methodology.</t>
-  </si>
-  <si>
-    <t>If there is no comparator, then there is no modification of the value</t>
-  </si>
-  <si>
-    <t>How the Quantity should be understood and represented.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/quantity-comparator|4.0.1</t>
-  </si>
-  <si>
-    <t>Quantity.comparator</t>
-  </si>
-  <si>
-    <t>SN.1  / CQ.1</t>
-  </si>
-  <si>
-    <t>IVL properties</t>
-  </si>
-  <si>
-    <t>Observation.value[x].unit</t>
-  </si>
-  <si>
-    <t>Unit representation</t>
-  </si>
-  <si>
-    <t>A human-readable form of the unit.</t>
-  </si>
-  <si>
-    <t>There are many representations for units of measure and in many contexts, particular representations are fixed and required. I.e. mcg for micrograms.</t>
-  </si>
-  <si>
-    <t>Quantity.unit</t>
-  </si>
-  <si>
-    <t>(see OBX.6 etc.) / CQ.2</t>
-  </si>
-  <si>
-    <t>PQ.unit</t>
-  </si>
-  <si>
-    <t>Observation.value[x].system</t>
-  </si>
-  <si>
-    <t>System that defines coded unit form</t>
-  </si>
-  <si>
-    <t>The identification of the system that provides the coded form of the unit.</t>
-  </si>
-  <si>
-    <t>Need to know the system that defines the coded form of the unit.</t>
-  </si>
-  <si>
-    <t>Quantity.system</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qty-3
-</t>
-  </si>
-  <si>
-    <t>CO.codeSystem, PQ.translation.codeSystem</t>
-  </si>
-  <si>
-    <t>Observation.value[x].code</t>
-  </si>
-  <si>
-    <t>Coded form of the unit</t>
-  </si>
-  <si>
-    <t>A computer processable form of the unit in some unit representation system.</t>
-  </si>
-  <si>
-    <t>The preferred system is UCUM, but SNOMED CT can also be used (for customary units) or ISO 4217 for currency.  The context of use may additionally require a code from a particular system.</t>
-  </si>
-  <si>
-    <t>Need a computable form of the unit that is fixed across all forms. UCUM provides this for quantities, but SNOMED CT provides many units of interest.</t>
-  </si>
-  <si>
-    <t>Quantity.code</t>
-  </si>
-  <si>
-    <t>PQ.code, MO.currency, PQ.translation.code</t>
+    <t>valueInteger</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1816,7 +1688,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO74"/>
+  <dimension ref="A1:AO67"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1849,7 +1721,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="51.1328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -6470,7 +6342,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6482,16 +6354,20 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>69</v>
+        <v>322</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>323</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6515,13 +6391,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>45</v>
+        <v>327</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6539,7 +6415,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>71</v>
+        <v>321</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6548,10 +6424,10 @@
         <v>55</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>45</v>
+        <v>328</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>45</v>
@@ -6560,10 +6436,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>155</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>72</v>
+        <v>329</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6574,18 +6450,18 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>74</v>
+        <v>331</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6597,18 +6473,20 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>75</v>
+        <v>204</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>76</v>
+        <v>332</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>77</v>
+        <v>333</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N41" s="2"/>
+        <v>334</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>335</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6632,31 +6510,31 @@
         <v>45</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>45</v>
+        <v>336</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>45</v>
+        <v>337</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="AC41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD41" t="s" s="2">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>82</v>
+        <v>330</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6668,30 +6546,30 @@
         <v>45</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>45</v>
+        <v>339</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>72</v>
+        <v>340</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>45</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6711,22 +6589,22 @@
         <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>324</v>
+        <v>343</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>325</v>
+        <v>344</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>326</v>
+        <v>345</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>328</v>
+        <v>347</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
@@ -6775,13 +6653,13 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>45</v>
@@ -6796,10 +6674,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6810,7 +6688,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>332</v>
+        <v>350</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6821,36 +6699,34 @@
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>132</v>
+        <v>204</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" t="s" s="2">
-        <v>335</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
-      <c r="P43" t="s" s="2">
-        <v>336</v>
-      </c>
+      <c r="P43" s="2"/>
       <c r="Q43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6870,13 +6746,13 @@
         <v>45</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>195</v>
+        <v>122</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>337</v>
+        <v>354</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>338</v>
+        <v>355</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>45</v>
@@ -6894,7 +6770,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6912,24 +6788,24 @@
         <v>45</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>45</v>
+        <v>356</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>340</v>
+        <v>357</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>341</v>
+        <v>358</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>45</v>
+        <v>359</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6949,20 +6825,22 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>343</v>
+        <v>361</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="M44" s="2"/>
+        <v>362</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>363</v>
+      </c>
       <c r="N44" t="s" s="2">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6987,13 +6865,13 @@
         <v>45</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>45</v>
+        <v>366</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>45</v>
@@ -7011,7 +6889,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -7032,10 +6910,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -7046,7 +6924,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7057,7 +6935,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -7066,21 +6944,21 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>97</v>
+        <v>370</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>350</v>
+        <v>371</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" t="s" s="2">
-        <v>352</v>
-      </c>
+        <v>372</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -7128,7 +7006,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>353</v>
+        <v>369</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -7137,7 +7015,7 @@
         <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>354</v>
+        <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>67</v>
@@ -7146,24 +7024,24 @@
         <v>45</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>45</v>
+        <v>374</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>347</v>
+        <v>375</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>355</v>
+        <v>376</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>45</v>
+        <v>377</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>356</v>
+        <v>378</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7174,7 +7052,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -7183,23 +7061,21 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>132</v>
+        <v>379</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>357</v>
+        <v>380</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>358</v>
+        <v>381</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -7247,7 +7123,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>361</v>
+        <v>378</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -7265,24 +7141,24 @@
         <v>45</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>45</v>
+        <v>383</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>347</v>
+        <v>384</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>45</v>
+        <v>386</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7305,19 +7181,19 @@
         <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>204</v>
+        <v>388</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>364</v>
+        <v>389</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>365</v>
+        <v>390</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>366</v>
+        <v>391</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>367</v>
+        <v>392</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7342,13 +7218,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>368</v>
+        <v>45</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>369</v>
+        <v>45</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -7366,19 +7242,19 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>363</v>
+        <v>387</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>370</v>
+        <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>67</v>
+        <v>393</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
@@ -7387,10 +7263,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>155</v>
+        <v>394</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7401,18 +7277,18 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>372</v>
+        <v>396</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>373</v>
+        <v>45</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
@@ -7424,20 +7300,16 @@
         <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>374</v>
+        <v>69</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>377</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7461,13 +7333,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>378</v>
+        <v>45</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>379</v>
+        <v>45</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7485,53 +7357,53 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>372</v>
+        <v>71</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>380</v>
+        <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>381</v>
+        <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>382</v>
+        <v>72</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>383</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>384</v>
+        <v>397</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
@@ -7543,20 +7415,18 @@
         <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>385</v>
+        <v>75</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>386</v>
+        <v>76</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>387</v>
+        <v>77</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>389</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7604,7 +7474,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>384</v>
+        <v>82</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7616,7 +7486,7 @@
         <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>45</v>
@@ -7625,10 +7495,10 @@
         <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>390</v>
+        <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>391</v>
+        <v>72</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
@@ -7639,41 +7509,43 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>45</v>
+        <v>399</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>204</v>
+        <v>75</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N50" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>402</v>
+      </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
       </c>
@@ -7697,13 +7569,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>397</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7721,42 +7593,42 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>398</v>
+        <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>399</v>
+        <v>45</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>400</v>
+        <v>155</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>401</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7767,7 +7639,7 @@
         <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
@@ -7779,20 +7651,16 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>204</v>
+        <v>405</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>406</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>45</v>
       </c>
@@ -7816,13 +7684,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>407</v>
+        <v>45</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>408</v>
+        <v>45</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7840,7 +7708,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7849,7 +7717,7 @@
         <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>408</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7886,7 +7754,7 @@
         <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>45</v>
@@ -7898,17 +7766,15 @@
         <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="K52" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="K52" t="s" s="2">
+      <c r="L52" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L52" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>415</v>
-      </c>
+      <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7966,7 +7832,7 @@
         <v>55</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>45</v>
+        <v>408</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>67</v>
@@ -7975,24 +7841,24 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>416</v>
+        <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>419</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8003,7 +7869,7 @@
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -8015,18 +7881,20 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>421</v>
+        <v>204</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="N53" s="2"/>
+        <v>418</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>419</v>
+      </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
       </c>
@@ -8050,13 +7918,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>45</v>
+        <v>136</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>45</v>
+        <v>420</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>45</v>
+        <v>421</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -8074,7 +7942,7 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
@@ -8092,24 +7960,24 @@
         <v>45</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>427</v>
+        <v>340</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>428</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8120,7 +7988,7 @@
         <v>43</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>45</v>
@@ -8132,19 +8000,19 @@
         <v>45</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>430</v>
+        <v>204</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>45</v>
@@ -8169,13 +8037,13 @@
         <v>45</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>45</v>
+        <v>429</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>45</v>
+        <v>430</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>45</v>
@@ -8193,7 +8061,7 @@
         <v>45</v>
       </c>
       <c r="AE54" t="s" s="2">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>43</v>
@@ -8205,19 +8073,19 @@
         <v>45</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>435</v>
+        <v>67</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>45</v>
+        <v>422</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>437</v>
+        <v>340</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>45</v>
@@ -8228,7 +8096,7 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8251,16 +8119,18 @@
         <v>45</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>57</v>
+        <v>432</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>69</v>
+        <v>433</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>70</v>
+        <v>434</v>
       </c>
       <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
+      <c r="N55" t="s" s="2">
+        <v>435</v>
+      </c>
       <c r="O55" t="s" s="2">
         <v>45</v>
       </c>
@@ -8308,7 +8178,7 @@
         <v>45</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>71</v>
+        <v>431</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>43</v>
@@ -8320,7 +8190,7 @@
         <v>45</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>45</v>
@@ -8332,7 +8202,7 @@
         <v>45</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>72</v>
+        <v>436</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>45</v>
@@ -8343,18 +8213,18 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>45</v>
@@ -8366,17 +8236,15 @@
         <v>45</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>76</v>
+        <v>438</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>45</v>
@@ -8425,19 +8293,19 @@
         <v>45</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>82</v>
+        <v>437</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>45</v>
@@ -8446,10 +8314,10 @@
         <v>45</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>45</v>
+        <v>409</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>72</v>
+        <v>440</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>45</v>
@@ -8460,43 +8328,41 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>441</v>
+        <v>45</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>75</v>
+        <v>442</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>444</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>45</v>
       </c>
@@ -8544,7 +8410,7 @@
         <v>45</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>43</v>
@@ -8556,7 +8422,7 @@
         <v>45</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>45</v>
@@ -8565,10 +8431,10 @@
         <v>45</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>45</v>
+        <v>446</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>155</v>
+        <v>447</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>45</v>
@@ -8579,7 +8445,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8590,7 +8456,7 @@
         <v>43</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>45</v>
@@ -8599,18 +8465,20 @@
         <v>45</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="M58" s="2"/>
+        <v>451</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>452</v>
+      </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>45</v>
@@ -8659,16 +8527,16 @@
         <v>45</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>450</v>
+        <v>45</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>67</v>
@@ -8680,10 +8548,10 @@
         <v>45</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>45</v>
@@ -8694,7 +8562,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8705,7 +8573,7 @@
         <v>43</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>45</v>
@@ -8714,19 +8582,23 @@
         <v>45</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>447</v>
+        <v>388</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>455</v>
-      </c>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
+        <v>456</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>458</v>
+      </c>
       <c r="O59" t="s" s="2">
         <v>45</v>
       </c>
@@ -8774,16 +8646,16 @@
         <v>45</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>450</v>
+        <v>45</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>67</v>
@@ -8795,10 +8667,10 @@
         <v>45</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>45</v>
@@ -8809,7 +8681,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8832,20 +8704,16 @@
         <v>45</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>204</v>
+        <v>57</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>458</v>
+        <v>69</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>459</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>460</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>461</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
         <v>45</v>
       </c>
@@ -8869,13 +8737,13 @@
         <v>45</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>462</v>
+        <v>45</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>463</v>
+        <v>45</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>45</v>
@@ -8893,7 +8761,7 @@
         <v>45</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>457</v>
+        <v>71</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>43</v>
@@ -8905,19 +8773,19 @@
         <v>45</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>464</v>
+        <v>45</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>465</v>
+        <v>45</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>382</v>
+        <v>72</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>45</v>
@@ -8928,11 +8796,11 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -8951,20 +8819,18 @@
         <v>45</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>204</v>
+        <v>75</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>467</v>
+        <v>76</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>468</v>
+        <v>77</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>469</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>470</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
         <v>45</v>
       </c>
@@ -8988,13 +8854,13 @@
         <v>45</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>471</v>
+        <v>45</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>472</v>
+        <v>45</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>45</v>
@@ -9012,7 +8878,7 @@
         <v>45</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>466</v>
+        <v>82</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>43</v>
@@ -9024,19 +8890,19 @@
         <v>45</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>464</v>
+        <v>45</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>465</v>
+        <v>45</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>382</v>
+        <v>72</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>45</v>
@@ -9047,40 +8913,42 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>45</v>
+        <v>399</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>474</v>
+        <v>75</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>475</v>
+        <v>400</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>476</v>
-      </c>
-      <c r="M62" s="2"/>
+        <v>401</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="N62" t="s" s="2">
-        <v>477</v>
+        <v>402</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>45</v>
@@ -9129,19 +8997,19 @@
         <v>45</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>473</v>
+        <v>403</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>45</v>
@@ -9153,7 +9021,7 @@
         <v>45</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>478</v>
+        <v>155</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>45</v>
@@ -9164,7 +9032,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9172,7 +9040,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F63" t="s" s="2">
         <v>55</v>
@@ -9184,19 +9052,23 @@
         <v>45</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>57</v>
+        <v>204</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>481</v>
-      </c>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
+        <v>466</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="N63" t="s" s="2">
+        <v>219</v>
+      </c>
       <c r="O63" t="s" s="2">
         <v>45</v>
       </c>
@@ -9220,13 +9092,13 @@
         <v>45</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>45</v>
+        <v>220</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>45</v>
+        <v>221</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>45</v>
@@ -9244,10 +9116,10 @@
         <v>45</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>55</v>
@@ -9262,16 +9134,16 @@
         <v>45</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>45</v>
+        <v>468</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>451</v>
+        <v>224</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>482</v>
+        <v>225</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>45</v>
+        <v>226</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>45</v>
@@ -9279,7 +9151,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9290,7 +9162,7 @@
         <v>43</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>45</v>
@@ -9302,18 +9174,20 @@
         <v>56</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>486</v>
+        <v>312</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="N64" s="2"/>
+        <v>472</v>
+      </c>
+      <c r="N64" t="s" s="2">
+        <v>314</v>
+      </c>
       <c r="O64" t="s" s="2">
         <v>45</v>
       </c>
@@ -9361,13 +9235,13 @@
         <v>45</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>45</v>
@@ -9379,24 +9253,24 @@
         <v>45</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>45</v>
+        <v>473</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>488</v>
+        <v>317</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>489</v>
+        <v>318</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO64" t="s" s="2">
-        <v>45</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9407,7 +9281,7 @@
         <v>43</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>45</v>
@@ -9416,21 +9290,23 @@
         <v>45</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>491</v>
+        <v>204</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>494</v>
-      </c>
-      <c r="N65" s="2"/>
+        <v>477</v>
+      </c>
+      <c r="N65" t="s" s="2">
+        <v>325</v>
+      </c>
       <c r="O65" t="s" s="2">
         <v>45</v>
       </c>
@@ -9454,13 +9330,13 @@
         <v>45</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>45</v>
+        <v>327</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>45</v>
@@ -9478,16 +9354,16 @@
         <v>45</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>45</v>
+        <v>328</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>67</v>
@@ -9499,10 +9375,10 @@
         <v>45</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>488</v>
+        <v>155</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>495</v>
+        <v>329</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>45</v>
@@ -9513,18 +9389,18 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>45</v>
+        <v>331</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>45</v>
@@ -9533,22 +9409,22 @@
         <v>45</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>430</v>
+        <v>204</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>497</v>
+        <v>332</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>498</v>
+        <v>333</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>499</v>
+        <v>334</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>500</v>
+        <v>335</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>45</v>
@@ -9573,13 +9449,13 @@
         <v>45</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>45</v>
+        <v>336</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>45</v>
+        <v>337</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>45</v>
@@ -9597,7 +9473,7 @@
         <v>45</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>496</v>
+        <v>478</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>43</v>
@@ -9615,24 +9491,24 @@
         <v>45</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>501</v>
+        <v>339</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>502</v>
+        <v>340</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>45</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9643,7 +9519,7 @@
         <v>43</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>45</v>
@@ -9655,16 +9531,20 @@
         <v>45</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>69</v>
+        <v>480</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
+        <v>481</v>
+      </c>
+      <c r="M67" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="N67" t="s" s="2">
+        <v>392</v>
+      </c>
       <c r="O67" t="s" s="2">
         <v>45</v>
       </c>
@@ -9712,19 +9592,19 @@
         <v>45</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>71</v>
+        <v>479</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG67" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>45</v>
@@ -9733,851 +9613,20 @@
         <v>45</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>45</v>
+        <v>394</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>72</v>
+        <v>395</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="68" hidden="true">
-      <c r="A68" t="s" s="2">
-        <v>504</v>
-      </c>
-      <c r="B68" s="2"/>
-      <c r="C68" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="D68" s="2"/>
-      <c r="E68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N68" s="2"/>
-      <c r="O68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P68" s="2"/>
-      <c r="Q68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="AN68" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO68" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" hidden="true">
-      <c r="A69" t="s" s="2">
-        <v>505</v>
-      </c>
-      <c r="B69" s="2"/>
-      <c r="C69" t="s" s="2">
-        <v>441</v>
-      </c>
-      <c r="D69" s="2"/>
-      <c r="E69" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H69" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="J69" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="K69" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>443</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>444</v>
-      </c>
-      <c r="O69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P69" s="2"/>
-      <c r="Q69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>445</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO69" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="70" hidden="true">
-      <c r="A70" t="s" s="2">
-        <v>506</v>
-      </c>
-      <c r="B70" s="2"/>
-      <c r="C70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D70" s="2"/>
-      <c r="E70" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="F70" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="G70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I70" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="J70" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="K70" t="s" s="2">
-        <v>507</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>509</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="O70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P70" s="2"/>
-      <c r="Q70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>506</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI70" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>510</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="AO70" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" hidden="true">
-      <c r="A71" t="s" s="2">
-        <v>511</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D71" s="2"/>
-      <c r="E71" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F71" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="G71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>56</v>
-      </c>
-      <c r="J71" t="s" s="2">
-        <v>512</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>513</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>514</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="O71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P71" s="2"/>
-      <c r="Q71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>511</v>
-      </c>
-      <c r="AF71" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="AN71" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO71" t="s" s="2">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="72" hidden="true">
-      <c r="A72" t="s" s="2">
-        <v>516</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D72" s="2"/>
-      <c r="E72" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F72" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>518</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>519</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>367</v>
-      </c>
-      <c r="O72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P72" s="2"/>
-      <c r="Q72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>368</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>516</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="AN72" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO72" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="73" hidden="true">
-      <c r="A73" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="D73" s="2"/>
-      <c r="E73" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>374</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="O73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P73" s="2"/>
-      <c r="Q73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO73" t="s" s="2">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="74" hidden="true">
-      <c r="A74" t="s" s="2">
-        <v>521</v>
-      </c>
-      <c r="B74" s="2"/>
-      <c r="C74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D74" s="2"/>
-      <c r="E74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>522</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>433</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>434</v>
-      </c>
-      <c r="O74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P74" s="2"/>
-      <c r="Q74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>521</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>436</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO74" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO74">
+  <autoFilter ref="A1:AO67">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10587,7 +9636,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI73">
+  <conditionalFormatting sqref="A2:AI66">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
change pain to valueQuantity
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-VA.MHV.pain.xlsx
+++ b/docs/StructureDefinition-VA.MHV.pain.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2539" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2800" uniqueCount="561">
   <si>
     <t>Property</t>
   </si>
@@ -87,6 +87,7 @@
 - must have vital-signs category
 - must have both LOINC#72514-3 and SCT#225908003 code
 - must have effectiveDateTime
+- must have valueQuantity with no units
   - must have integer between 0-10
 - must have status at final
 - must point at the patient
@@ -1112,7 +1113,7 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">integer
+    <t xml:space="preserve">Quantity
 </t>
   </si>
   <si>
@@ -1144,10 +1145,148 @@
     <t>363714003 |Interprets|</t>
   </si>
   <si>
-    <t>valueInteger</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>valueQuantity</t>
+  </si>
+  <si>
+    <t>Observation.value[x].id</t>
+  </si>
+  <si>
+    <t>Observation.value[x].extension</t>
+  </si>
+  <si>
+    <t>Observation.value[x].value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal
+</t>
+  </si>
+  <si>
+    <t>Numerical value (with implicit precision)</t>
+  </si>
+  <si>
+    <t>The value of the measured amount. The value includes an implicit precision in the presentation of the value.</t>
+  </si>
+  <si>
+    <t>The implicit precision in the value should always be honored. Monetary values have their own rules for handling precision (refer to standard accounting text books).</t>
+  </si>
+  <si>
+    <t>Precision is handled implicitly in almost all cases of measurement.</t>
+  </si>
+  <si>
+    <t>&lt;valueQuantity xmlns="http://hl7.org/fhir"&gt;
+  &lt;system value="http://unitsofmeasure.org"/&gt;
+  &lt;code value="{score}"/&gt;
+&lt;/valueQuantity&gt;</t>
+  </si>
+  <si>
+    <t>&lt;valueQuantity xmlns="http://hl7.org/fhir"&gt;
+  &lt;value value="10"/&gt;
+  &lt;system value="http://unitsofmeasure.org"/&gt;
+  &lt;code value="{score}"/&gt;
+&lt;/valueQuantity&gt;</t>
+  </si>
+  <si>
+    <t>Quantity.value</t>
+  </si>
+  <si>
+    <t>SN.2  / CQ - N/A</t>
+  </si>
+  <si>
+    <t>PQ.value, CO.value, MO.value, IVL.high or IVL.low depending on the value</t>
+  </si>
+  <si>
+    <t>Observation.value[x].comparator</t>
+  </si>
+  <si>
+    <t>&lt; | &lt;= | &gt;= | &gt; - how to understand the value</t>
+  </si>
+  <si>
+    <t>How the value should be understood and represented - whether the actual value is greater or less than the stated value due to measurement issues; e.g. if the comparator is "&lt;" , then the real value is &lt; stated value.</t>
+  </si>
+  <si>
+    <t>Need a framework for handling measures where the value is &lt;5ug/L or &gt;400mg/L due to the limitations of measuring methodology.</t>
+  </si>
+  <si>
+    <t>If there is no comparator, then there is no modification of the value</t>
+  </si>
+  <si>
+    <t>How the Quantity should be understood and represented.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/quantity-comparator|4.0.1</t>
+  </si>
+  <si>
+    <t>Quantity.comparator</t>
+  </si>
+  <si>
+    <t>SN.1  / CQ.1</t>
+  </si>
+  <si>
+    <t>IVL properties</t>
+  </si>
+  <si>
+    <t>Observation.value[x].unit</t>
+  </si>
+  <si>
+    <t>Unit representation</t>
+  </si>
+  <si>
+    <t>A human-readable form of the unit.</t>
+  </si>
+  <si>
+    <t>There are many representations for units of measure and in many contexts, particular representations are fixed and required. I.e. mcg for micrograms.</t>
+  </si>
+  <si>
+    <t>Quantity.unit</t>
+  </si>
+  <si>
+    <t>(see OBX.6 etc.) / CQ.2</t>
+  </si>
+  <si>
+    <t>PQ.unit</t>
+  </si>
+  <si>
+    <t>Observation.value[x].system</t>
+  </si>
+  <si>
+    <t>System that defines coded unit form</t>
+  </si>
+  <si>
+    <t>The identification of the system that provides the coded form of the unit.</t>
+  </si>
+  <si>
+    <t>Need to know the system that defines the coded form of the unit.</t>
+  </si>
+  <si>
+    <t>Quantity.system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qty-3
+</t>
+  </si>
+  <si>
+    <t>CO.codeSystem, PQ.translation.codeSystem</t>
+  </si>
+  <si>
+    <t>Observation.value[x].code</t>
+  </si>
+  <si>
+    <t>Coded form of the unit</t>
+  </si>
+  <si>
+    <t>A computer processable form of the unit in some unit representation system.</t>
+  </si>
+  <si>
+    <t>The preferred system is UCUM, but SNOMED CT can also be used (for customary units) or ISO 4217 for currency.  The context of use may additionally require a code from a particular system.</t>
+  </si>
+  <si>
+    <t>Need a computable form of the unit that is fixed across all forms. UCUM provides this for quantities, but SNOMED CT provides many units of interest.</t>
+  </si>
+  <si>
+    <t>Quantity.code</t>
+  </si>
+  <si>
+    <t>PQ.code, MO.currency, PQ.translation.code</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1960,7 +2099,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO67"/>
+  <dimension ref="A1:AO74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1988,12 +2127,12 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7109375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="43.15625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="43.15625" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.7734375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="51.1328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -6535,10 +6674,10 @@
         <v>80</v>
       </c>
       <c r="T39" t="s" s="2">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="U39" t="s" s="2">
-        <v>356</v>
+        <v>80</v>
       </c>
       <c r="V39" t="s" s="2">
         <v>80</v>
@@ -6603,7 +6742,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6614,7 +6753,7 @@
         <v>78</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>80</v>
@@ -6626,20 +6765,16 @@
         <v>80</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>361</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>80</v>
       </c>
@@ -6663,13 +6798,13 @@
         <v>80</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>362</v>
+        <v>80</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>363</v>
+        <v>80</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>80</v>
@@ -6687,7 +6822,7 @@
         <v>80</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>357</v>
+        <v>106</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>78</v>
@@ -6696,10 +6831,10 @@
         <v>90</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>364</v>
+        <v>80</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>80</v>
@@ -6708,10 +6843,10 @@
         <v>80</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>190</v>
+        <v>80</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>365</v>
+        <v>107</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>80</v>
@@ -6722,18 +6857,18 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
-        <v>367</v>
+        <v>109</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>80</v>
@@ -6745,20 +6880,18 @@
         <v>80</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>239</v>
+        <v>110</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>368</v>
+        <v>111</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>369</v>
+        <v>112</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>371</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>80</v>
       </c>
@@ -6782,31 +6915,31 @@
         <v>80</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>372</v>
+        <v>80</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>373</v>
+        <v>80</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AA41" t="s" s="2">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="AC41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AD41" t="s" s="2">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>366</v>
+        <v>117</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>78</v>
@@ -6818,30 +6951,30 @@
         <v>80</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AJ41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>374</v>
+        <v>80</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>375</v>
+        <v>80</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>376</v>
+        <v>107</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>377</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6861,22 +6994,22 @@
         <v>80</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>383</v>
+        <v>363</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>80</v>
@@ -6892,10 +7025,10 @@
         <v>80</v>
       </c>
       <c r="T42" t="s" s="2">
-        <v>80</v>
+        <v>364</v>
       </c>
       <c r="U42" t="s" s="2">
-        <v>80</v>
+        <v>365</v>
       </c>
       <c r="V42" t="s" s="2">
         <v>80</v>
@@ -6925,13 +7058,13 @@
         <v>80</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>80</v>
@@ -6946,10 +7079,10 @@
         <v>80</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>385</v>
+        <v>368</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>80</v>
@@ -6960,7 +7093,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>386</v>
+        <v>369</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6971,34 +7104,36 @@
         <v>78</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>239</v>
+        <v>167</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>387</v>
+        <v>370</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="N43" s="2"/>
+        <v>371</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" t="s" s="2">
+        <v>372</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="P43" s="2"/>
+      <c r="P43" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="Q43" t="s" s="2">
         <v>80</v>
       </c>
@@ -7018,13 +7153,13 @@
         <v>80</v>
       </c>
       <c r="W43" t="s" s="2">
-        <v>157</v>
+        <v>230</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="Z43" t="s" s="2">
         <v>80</v>
@@ -7042,7 +7177,7 @@
         <v>80</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>78</v>
@@ -7060,24 +7195,24 @@
         <v>80</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>392</v>
+        <v>80</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>395</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>396</v>
+        <v>379</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -7088,7 +7223,7 @@
         <v>78</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>80</v>
@@ -7097,22 +7232,20 @@
         <v>80</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>397</v>
+        <v>380</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>398</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>399</v>
-      </c>
+        <v>381</v>
+      </c>
+      <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>80</v>
@@ -7137,13 +7270,13 @@
         <v>80</v>
       </c>
       <c r="W44" t="s" s="2">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="X44" t="s" s="2">
-        <v>401</v>
+        <v>80</v>
       </c>
       <c r="Y44" t="s" s="2">
-        <v>402</v>
+        <v>80</v>
       </c>
       <c r="Z44" t="s" s="2">
         <v>80</v>
@@ -7161,7 +7294,7 @@
         <v>80</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>78</v>
@@ -7182,10 +7315,10 @@
         <v>80</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>404</v>
+        <v>385</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>80</v>
@@ -7196,7 +7329,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -7207,7 +7340,7 @@
         <v>78</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>80</v>
@@ -7216,21 +7349,21 @@
         <v>80</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>406</v>
+        <v>132</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>388</v>
+      </c>
+      <c r="M45" s="2"/>
+      <c r="N45" t="s" s="2">
+        <v>389</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>80</v>
       </c>
@@ -7278,7 +7411,7 @@
         <v>80</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>78</v>
@@ -7287,7 +7420,7 @@
         <v>90</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>80</v>
+        <v>391</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>102</v>
@@ -7296,24 +7429,24 @@
         <v>80</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>410</v>
+        <v>80</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>411</v>
+        <v>384</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>412</v>
+        <v>392</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>413</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -7324,7 +7457,7 @@
         <v>78</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>80</v>
@@ -7333,21 +7466,23 @@
         <v>80</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>415</v>
+        <v>167</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>417</v>
+        <v>395</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="N46" s="2"/>
+        <v>396</v>
+      </c>
+      <c r="N46" t="s" s="2">
+        <v>397</v>
+      </c>
       <c r="O46" t="s" s="2">
         <v>80</v>
       </c>
@@ -7395,7 +7530,7 @@
         <v>80</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>78</v>
@@ -7413,24 +7548,24 @@
         <v>80</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>419</v>
+        <v>80</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>420</v>
+        <v>384</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>421</v>
+        <v>399</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO46" t="s" s="2">
-        <v>422</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7453,19 +7588,19 @@
         <v>80</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>424</v>
+        <v>239</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>425</v>
+        <v>401</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>428</v>
+        <v>404</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>80</v>
@@ -7490,13 +7625,13 @@
         <v>80</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>80</v>
+        <v>405</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>80</v>
+        <v>406</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>80</v>
@@ -7514,19 +7649,19 @@
         <v>80</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>80</v>
+        <v>407</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>429</v>
+        <v>102</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>80</v>
@@ -7535,10 +7670,10 @@
         <v>80</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>430</v>
+        <v>190</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>80</v>
@@ -7549,18 +7684,18 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>80</v>
+        <v>410</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>80</v>
@@ -7572,16 +7707,20 @@
         <v>80</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>92</v>
+        <v>239</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>104</v>
+        <v>411</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+        <v>412</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>414</v>
+      </c>
       <c r="O48" t="s" s="2">
         <v>80</v>
       </c>
@@ -7605,13 +7744,13 @@
         <v>80</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>80</v>
+        <v>415</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>80</v>
+        <v>416</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>80</v>
@@ -7629,53 +7768,53 @@
         <v>80</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>106</v>
+        <v>409</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>80</v>
+        <v>417</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>80</v>
+        <v>418</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>107</v>
+        <v>419</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>80</v>
+        <v>420</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>80</v>
@@ -7687,18 +7826,20 @@
         <v>80</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>110</v>
+        <v>422</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>111</v>
+        <v>423</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>112</v>
+        <v>424</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N49" s="2"/>
+        <v>425</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>426</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>80</v>
       </c>
@@ -7746,7 +7887,7 @@
         <v>80</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>117</v>
+        <v>421</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>78</v>
@@ -7758,7 +7899,7 @@
         <v>80</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>80</v>
@@ -7767,10 +7908,10 @@
         <v>80</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>80</v>
+        <v>427</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>107</v>
+        <v>428</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>80</v>
@@ -7781,43 +7922,41 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>435</v>
+        <v>80</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>110</v>
+        <v>239</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>438</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
         <v>80</v>
       </c>
@@ -7841,13 +7980,13 @@
         <v>80</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>80</v>
+        <v>433</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>80</v>
+        <v>434</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>80</v>
@@ -7865,42 +8004,42 @@
         <v>80</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>80</v>
+        <v>435</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>80</v>
+        <v>436</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>190</v>
+        <v>437</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>80</v>
+        <v>438</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7911,7 +8050,7 @@
         <v>78</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>80</v>
@@ -7923,16 +8062,20 @@
         <v>80</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="N51" t="s" s="2">
         <v>443</v>
       </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
       <c r="O51" t="s" s="2">
         <v>80</v>
       </c>
@@ -7956,13 +8099,13 @@
         <v>80</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>80</v>
+        <v>444</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>80</v>
+        <v>445</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>80</v>
@@ -7980,7 +8123,7 @@
         <v>80</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>78</v>
@@ -7989,7 +8132,7 @@
         <v>90</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>444</v>
+        <v>80</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>102</v>
@@ -8001,10 +8144,10 @@
         <v>80</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>80</v>
@@ -8015,7 +8158,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -8026,7 +8169,7 @@
         <v>78</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>80</v>
@@ -8038,15 +8181,17 @@
         <v>80</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="M52" s="2"/>
+        <v>451</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>452</v>
+      </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
         <v>80</v>
@@ -8095,7 +8240,7 @@
         <v>80</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>78</v>
@@ -8104,7 +8249,7 @@
         <v>90</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>444</v>
+        <v>80</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>102</v>
@@ -8113,24 +8258,24 @@
         <v>80</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>80</v>
+        <v>453</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>80</v>
+        <v>456</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -8141,7 +8286,7 @@
         <v>78</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>80</v>
@@ -8153,20 +8298,18 @@
         <v>80</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>239</v>
+        <v>458</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>454</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>455</v>
-      </c>
+        <v>461</v>
+      </c>
+      <c r="N53" s="2"/>
       <c r="O53" t="s" s="2">
         <v>80</v>
       </c>
@@ -8190,31 +8333,31 @@
         <v>80</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>456</v>
+        <v>80</v>
       </c>
       <c r="Y53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE53" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>451</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>78</v>
@@ -8232,24 +8375,24 @@
         <v>80</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>376</v>
+        <v>464</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>80</v>
+        <v>465</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -8260,7 +8403,7 @@
         <v>78</v>
       </c>
       <c r="F54" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G54" t="s" s="2">
         <v>80</v>
@@ -8272,19 +8415,19 @@
         <v>80</v>
       </c>
       <c r="J54" t="s" s="2">
-        <v>239</v>
+        <v>467</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="O54" t="s" s="2">
         <v>80</v>
@@ -8309,31 +8452,31 @@
         <v>80</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>465</v>
+        <v>80</v>
       </c>
       <c r="Y54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE54" t="s" s="2">
         <v>466</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>460</v>
       </c>
       <c r="AF54" t="s" s="2">
         <v>78</v>
@@ -8345,19 +8488,19 @@
         <v>80</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>102</v>
+        <v>472</v>
       </c>
       <c r="AJ54" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>458</v>
+        <v>80</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>459</v>
+        <v>473</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>376</v>
+        <v>474</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>80</v>
@@ -8368,7 +8511,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -8391,18 +8534,16 @@
         <v>80</v>
       </c>
       <c r="J55" t="s" s="2">
-        <v>468</v>
+        <v>92</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>469</v>
+        <v>104</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>470</v>
+        <v>105</v>
       </c>
       <c r="M55" s="2"/>
-      <c r="N55" t="s" s="2">
-        <v>471</v>
-      </c>
+      <c r="N55" s="2"/>
       <c r="O55" t="s" s="2">
         <v>80</v>
       </c>
@@ -8450,7 +8591,7 @@
         <v>80</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>467</v>
+        <v>106</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>78</v>
@@ -8462,7 +8603,7 @@
         <v>80</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>80</v>
@@ -8474,7 +8615,7 @@
         <v>80</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>472</v>
+        <v>107</v>
       </c>
       <c r="AN55" t="s" s="2">
         <v>80</v>
@@ -8485,18 +8626,18 @@
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F56" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>80</v>
@@ -8508,15 +8649,17 @@
         <v>80</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>474</v>
+        <v>111</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>475</v>
-      </c>
-      <c r="M56" s="2"/>
+        <v>112</v>
+      </c>
+      <c r="M56" t="s" s="2">
+        <v>113</v>
+      </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
         <v>80</v>
@@ -8565,19 +8708,19 @@
         <v>80</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>473</v>
+        <v>117</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>80</v>
@@ -8586,10 +8729,10 @@
         <v>80</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>445</v>
+        <v>80</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>476</v>
+        <v>107</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>80</v>
@@ -8604,26 +8747,26 @@
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>80</v>
+        <v>478</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F57" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G57" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>91</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>478</v>
+        <v>110</v>
       </c>
       <c r="K57" t="s" s="2">
         <v>479</v>
@@ -8632,9 +8775,11 @@
         <v>480</v>
       </c>
       <c r="M57" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="N57" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
         <v>80</v>
       </c>
@@ -8682,7 +8827,7 @@
         <v>80</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>78</v>
@@ -8694,7 +8839,7 @@
         <v>80</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>80</v>
@@ -8703,10 +8848,10 @@
         <v>80</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>482</v>
+        <v>80</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>483</v>
+        <v>190</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>80</v>
@@ -8717,7 +8862,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8728,7 +8873,7 @@
         <v>78</v>
       </c>
       <c r="F58" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G58" t="s" s="2">
         <v>80</v>
@@ -8737,20 +8882,18 @@
         <v>80</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>484</v>
+      </c>
+      <c r="K58" t="s" s="2">
         <v>485</v>
       </c>
-      <c r="K58" t="s" s="2">
+      <c r="L58" t="s" s="2">
         <v>486</v>
       </c>
-      <c r="L58" t="s" s="2">
-        <v>487</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>488</v>
-      </c>
+      <c r="M58" s="2"/>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
         <v>80</v>
@@ -8799,16 +8942,16 @@
         <v>80</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG58" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>80</v>
+        <v>487</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>102</v>
@@ -8820,7 +8963,7 @@
         <v>80</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>489</v>
@@ -8845,7 +8988,7 @@
         <v>78</v>
       </c>
       <c r="F59" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G59" t="s" s="2">
         <v>80</v>
@@ -8854,10 +8997,10 @@
         <v>80</v>
       </c>
       <c r="I59" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J59" t="s" s="2">
-        <v>424</v>
+        <v>484</v>
       </c>
       <c r="K59" t="s" s="2">
         <v>491</v>
@@ -8865,12 +9008,8 @@
       <c r="L59" t="s" s="2">
         <v>492</v>
       </c>
-      <c r="M59" t="s" s="2">
-        <v>493</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>494</v>
-      </c>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
         <v>80</v>
       </c>
@@ -8924,10 +9063,10 @@
         <v>78</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>80</v>
+        <v>487</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>102</v>
@@ -8939,10 +9078,10 @@
         <v>80</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>80</v>
@@ -8953,7 +9092,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8976,16 +9115,20 @@
         <v>80</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>92</v>
+        <v>239</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>104</v>
+        <v>495</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
+        <v>496</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>497</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>498</v>
+      </c>
       <c r="O60" t="s" s="2">
         <v>80</v>
       </c>
@@ -9009,13 +9152,13 @@
         <v>80</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>80</v>
+        <v>499</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>80</v>
+        <v>500</v>
       </c>
       <c r="Z60" t="s" s="2">
         <v>80</v>
@@ -9033,7 +9176,7 @@
         <v>80</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>106</v>
+        <v>494</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>78</v>
@@ -9045,19 +9188,19 @@
         <v>80</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ60" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>80</v>
+        <v>501</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>107</v>
+        <v>419</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>80</v>
@@ -9068,11 +9211,11 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -9091,18 +9234,20 @@
         <v>80</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>110</v>
+        <v>239</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>111</v>
+        <v>504</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>112</v>
+        <v>505</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N61" s="2"/>
+        <v>506</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>507</v>
+      </c>
       <c r="O61" t="s" s="2">
         <v>80</v>
       </c>
@@ -9126,13 +9271,13 @@
         <v>80</v>
       </c>
       <c r="W61" t="s" s="2">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>80</v>
+        <v>508</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>80</v>
+        <v>509</v>
       </c>
       <c r="Z61" t="s" s="2">
         <v>80</v>
@@ -9150,7 +9295,7 @@
         <v>80</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>117</v>
+        <v>503</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>78</v>
@@ -9162,19 +9307,19 @@
         <v>80</v>
       </c>
       <c r="AI61" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AJ61" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>80</v>
+        <v>501</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>80</v>
+        <v>502</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>107</v>
+        <v>419</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>80</v>
@@ -9185,42 +9330,40 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
-        <v>435</v>
+        <v>80</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F62" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G62" t="s" s="2">
         <v>80</v>
       </c>
       <c r="H62" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I62" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>110</v>
+        <v>511</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>436</v>
+        <v>512</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>113</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="M62" s="2"/>
       <c r="N62" t="s" s="2">
-        <v>438</v>
+        <v>514</v>
       </c>
       <c r="O62" t="s" s="2">
         <v>80</v>
@@ -9269,19 +9412,19 @@
         <v>80</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>439</v>
+        <v>510</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG62" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH62" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="AJ62" t="s" s="2">
         <v>80</v>
@@ -9293,7 +9436,7 @@
         <v>80</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>190</v>
+        <v>515</v>
       </c>
       <c r="AN62" t="s" s="2">
         <v>80</v>
@@ -9304,7 +9447,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -9312,7 +9455,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F63" t="s" s="2">
         <v>90</v>
@@ -9324,23 +9467,19 @@
         <v>80</v>
       </c>
       <c r="I63" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J63" t="s" s="2">
-        <v>239</v>
+        <v>92</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>502</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="N63" t="s" s="2">
-        <v>254</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
         <v>80</v>
       </c>
@@ -9364,13 +9503,13 @@
         <v>80</v>
       </c>
       <c r="W63" t="s" s="2">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="Y63" t="s" s="2">
-        <v>256</v>
+        <v>80</v>
       </c>
       <c r="Z63" t="s" s="2">
         <v>80</v>
@@ -9388,10 +9527,10 @@
         <v>80</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>500</v>
+        <v>516</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>90</v>
@@ -9406,16 +9545,16 @@
         <v>80</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>504</v>
+        <v>80</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>259</v>
+        <v>488</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>260</v>
+        <v>519</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>261</v>
+        <v>80</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>80</v>
@@ -9423,7 +9562,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>505</v>
+        <v>520</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -9434,7 +9573,7 @@
         <v>78</v>
       </c>
       <c r="F64" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G64" t="s" s="2">
         <v>80</v>
@@ -9446,20 +9585,18 @@
         <v>91</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>506</v>
+        <v>521</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>507</v>
+        <v>522</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>347</v>
+        <v>523</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>508</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>349</v>
-      </c>
+        <v>524</v>
+      </c>
+      <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
         <v>80</v>
       </c>
@@ -9507,13 +9644,13 @@
         <v>80</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>505</v>
+        <v>520</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG64" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH64" t="s" s="2">
         <v>80</v>
@@ -9525,24 +9662,24 @@
         <v>80</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>509</v>
+        <v>80</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>352</v>
+        <v>525</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>353</v>
+        <v>526</v>
       </c>
       <c r="AN64" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO64" t="s" s="2">
-        <v>354</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>510</v>
+        <v>527</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -9553,7 +9690,7 @@
         <v>78</v>
       </c>
       <c r="F65" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>80</v>
@@ -9562,23 +9699,21 @@
         <v>80</v>
       </c>
       <c r="I65" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J65" t="s" s="2">
-        <v>239</v>
+        <v>528</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>513</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>361</v>
-      </c>
+        <v>531</v>
+      </c>
+      <c r="N65" s="2"/>
       <c r="O65" t="s" s="2">
         <v>80</v>
       </c>
@@ -9602,13 +9737,13 @@
         <v>80</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="X65" t="s" s="2">
-        <v>362</v>
+        <v>80</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>363</v>
+        <v>80</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>80</v>
@@ -9626,16 +9761,16 @@
         <v>80</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>510</v>
+        <v>527</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>364</v>
+        <v>80</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>102</v>
@@ -9647,10 +9782,10 @@
         <v>80</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>190</v>
+        <v>525</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>365</v>
+        <v>532</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>80</v>
@@ -9661,18 +9796,18 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>514</v>
+        <v>533</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
-        <v>367</v>
+        <v>80</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" t="s" s="2">
         <v>78</v>
       </c>
       <c r="F66" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G66" t="s" s="2">
         <v>80</v>
@@ -9681,22 +9816,22 @@
         <v>80</v>
       </c>
       <c r="I66" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>239</v>
+        <v>467</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>368</v>
+        <v>534</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>369</v>
+        <v>535</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>370</v>
+        <v>536</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>371</v>
+        <v>537</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>80</v>
@@ -9721,13 +9856,13 @@
         <v>80</v>
       </c>
       <c r="W66" t="s" s="2">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>372</v>
+        <v>80</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>373</v>
+        <v>80</v>
       </c>
       <c r="Z66" t="s" s="2">
         <v>80</v>
@@ -9745,7 +9880,7 @@
         <v>80</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>514</v>
+        <v>533</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>78</v>
@@ -9763,24 +9898,24 @@
         <v>80</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>374</v>
+        <v>80</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>375</v>
+        <v>538</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>376</v>
+        <v>539</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AO66" t="s" s="2">
-        <v>377</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>515</v>
+        <v>540</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9791,7 +9926,7 @@
         <v>78</v>
       </c>
       <c r="F67" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G67" t="s" s="2">
         <v>80</v>
@@ -9803,20 +9938,16 @@
         <v>80</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>516</v>
+        <v>104</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>428</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
         <v>80</v>
       </c>
@@ -9864,36 +9995,867 @@
         <v>80</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>515</v>
+        <v>106</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AG67" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM67" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AN67" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO67" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="2">
+        <v>541</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F68" t="s" s="2">
         <v>79</v>
       </c>
-      <c r="AH67" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AI67" t="s" s="2">
+      <c r="G68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J68" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="K68" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="N68" s="2"/>
+      <c r="O68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P68" s="2"/>
+      <c r="Q68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE68" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="AF68" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG68" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI68" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AJ68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM68" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="AN68" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO68" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="2">
+        <v>542</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F69" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H69" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="I69" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="J69" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="K69" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="L69" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="O69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P69" s="2"/>
+      <c r="Q69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AF69" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG69" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI69" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AJ69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM69" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="AN69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO69" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="F70" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="G70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I70" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="J70" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K70" t="s" s="2">
+        <v>544</v>
+      </c>
+      <c r="L70" t="s" s="2">
+        <v>545</v>
+      </c>
+      <c r="M70" t="s" s="2">
+        <v>546</v>
+      </c>
+      <c r="N70" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="O70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P70" s="2"/>
+      <c r="Q70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W70" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="X70" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y70" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="Z70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE70" t="s" s="2">
+        <v>543</v>
+      </c>
+      <c r="AF70" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AG70" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI70" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="AJ67" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>430</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AO67" t="s" s="2">
+      <c r="AJ70" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK70" t="s" s="2">
+        <v>547</v>
+      </c>
+      <c r="AL70" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="AM70" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="AN70" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AO70" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F71" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="G71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I71" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="J71" t="s" s="2">
+        <v>549</v>
+      </c>
+      <c r="K71" t="s" s="2">
+        <v>550</v>
+      </c>
+      <c r="L71" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="M71" t="s" s="2">
+        <v>551</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="O71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P71" s="2"/>
+      <c r="Q71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE71" t="s" s="2">
+        <v>548</v>
+      </c>
+      <c r="AF71" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG71" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI71" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK71" t="s" s="2">
+        <v>552</v>
+      </c>
+      <c r="AL71" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AM71" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="AN71" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO71" t="s" s="2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F72" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="G72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J72" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K72" t="s" s="2">
+        <v>554</v>
+      </c>
+      <c r="L72" t="s" s="2">
+        <v>555</v>
+      </c>
+      <c r="M72" t="s" s="2">
+        <v>556</v>
+      </c>
+      <c r="N72" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="O72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P72" s="2"/>
+      <c r="Q72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W72" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="X72" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="Y72" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="Z72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE72" t="s" s="2">
+        <v>553</v>
+      </c>
+      <c r="AF72" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG72" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH72" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="AI72" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL72" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="AM72" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AN72" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO72" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F73" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J73" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="K73" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L73" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M73" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="N73" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="O73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P73" s="2"/>
+      <c r="Q73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W73" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="X73" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="Y73" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="Z73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE73" t="s" s="2">
+        <v>557</v>
+      </c>
+      <c r="AF73" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG73" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI73" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="AM73" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="AN73" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO73" t="s" s="2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="D74" s="2"/>
+      <c r="E74" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="F74" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K74" t="s" s="2">
+        <v>559</v>
+      </c>
+      <c r="L74" t="s" s="2">
+        <v>560</v>
+      </c>
+      <c r="M74" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="N74" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="O74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="P74" s="2"/>
+      <c r="Q74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="R74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE74" t="s" s="2">
+        <v>558</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL74" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="AM74" t="s" s="2">
+        <v>474</v>
+      </c>
+      <c r="AN74" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO74" t="s" s="2">
         <v>80</v>
       </c>
     </row>

</xml_diff>